<commit_message>
Altered Template and placed other files needed
</commit_message>
<xml_diff>
--- a/Errors.xlsx
+++ b/Errors.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ERROS</t>
   </si>
@@ -104,6 +104,15 @@
   <si>
     <t>http://stackoverflow.com/questions/22861077/django-auth-with-mongoengine-db</t>
   </si>
+  <si>
+    <t>Invalid block tag on line 10: 'static'. Did you forget to register or load this tag?</t>
+  </si>
+  <si>
+    <t>Add {% load staticfiles %} at the top of the html page.</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/27886477/invalid-block-tag-static</t>
+  </si>
 </sst>
 </file>
 
@@ -112,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -147,11 +156,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,7 +217,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,10 +238,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="87.3"/>
@@ -317,6 +321,17 @@
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="101.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>